<commit_message>
refreshing bug export and MFT summary
</commit_message>
<xml_diff>
--- a/issues/Scripted_MFT.xlsx
+++ b/issues/Scripted_MFT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\meng-ucalgary\seng-637-assignment-1\issues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34847A89-22EB-4AE1-AF98-9211F8C04AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC96CB4-CCA3-495D-82FB-B9D14DFA478B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="157">
   <si>
     <t>Use Case</t>
   </si>
@@ -451,9 +451,6 @@
     <t>No bug</t>
   </si>
   <si>
-    <t>Not yet logged</t>
-  </si>
-  <si>
     <t>Bug found during exploratory testing as well.</t>
   </si>
   <si>
@@ -504,12 +501,18 @@
   <si>
     <t>Output displayed as expected. However during input, the bug in #14 has to be kept in mind.</t>
   </si>
+  <si>
+    <t>https://seng637g5.backlog.com/view/ATM_1-25</t>
+  </si>
+  <si>
+    <t>https://seng637g5.backlog.com/view/ATM_1-26</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,12 +522,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -560,9 +557,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -573,16 +570,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1389,34 +1383,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>135</v>
       </c>
       <c r="K1" s="2"/>
@@ -1466,7 +1460,7 @@
         <v>137</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -1506,16 +1500,16 @@
         <v>15</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>151</v>
+      <c r="J3" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -1535,7 +1529,7 @@
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
     </row>
-    <row r="4" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1555,15 +1549,15 @@
         <v>19</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="J4" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>136</v>
       </c>
       <c r="K4" s="2"/>
@@ -1613,7 +1607,7 @@
         <v>137</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -1662,7 +1656,7 @@
         <v>137</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1702,16 +1696,16 @@
         <v>30</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>138</v>
+        <v>152</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -1760,7 +1754,7 @@
         <v>137</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1809,7 +1803,7 @@
         <v>137</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -1858,7 +1852,7 @@
         <v>137</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1907,7 +1901,7 @@
         <v>137</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -1927,7 +1921,7 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1956,7 +1950,7 @@
         <v>137</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -2005,7 +1999,7 @@
         <v>137</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -2051,10 +2045,10 @@
         <v>59</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>138</v>
+        <v>152</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>156</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -2100,10 +2094,10 @@
         <v>11</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>141</v>
+        <v>152</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -2152,7 +2146,7 @@
         <v>137</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -2192,7 +2186,7 @@
         <v>72</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>11</v>
@@ -2201,7 +2195,7 @@
         <v>137</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -2250,7 +2244,7 @@
         <v>137</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -2299,7 +2293,7 @@
         <v>137</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -2348,7 +2342,7 @@
         <v>137</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -2397,7 +2391,7 @@
         <v>137</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -2446,7 +2440,7 @@
         <v>137</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -2492,10 +2486,10 @@
         <v>132</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -2515,7 +2509,7 @@
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
     </row>
-    <row r="24" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2544,7 +2538,7 @@
         <v>137</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
@@ -2564,7 +2558,7 @@
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
     </row>
-    <row r="25" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -2593,7 +2587,7 @@
         <v>137</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -2613,7 +2607,7 @@
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
     </row>
-    <row r="26" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -2642,7 +2636,7 @@
         <v>137</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -2691,7 +2685,7 @@
         <v>137</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -2740,7 +2734,7 @@
         <v>137</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -2789,7 +2783,7 @@
         <v>137</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
@@ -2829,16 +2823,16 @@
         <v>105</v>
       </c>
       <c r="G30" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="I30" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J30" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -2887,7 +2881,7 @@
         <v>137</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
@@ -2936,7 +2930,7 @@
         <v>137</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -2985,7 +2979,7 @@
         <v>137</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -3034,7 +3028,7 @@
         <v>137</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -3083,7 +3077,7 @@
         <v>137</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -3132,7 +3126,7 @@
         <v>137</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -3152,7 +3146,7 @@
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
     </row>
-    <row r="37" spans="1:27" ht="72" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -3181,7 +3175,7 @@
         <v>137</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -3221,16 +3215,16 @@
         <v>122</v>
       </c>
       <c r="G38" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J38" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J38" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -3279,7 +3273,7 @@
         <v>137</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -3319,16 +3313,16 @@
         <v>122</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J40" s="7" t="s">
-        <v>148</v>
+        <v>138</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -3348,7 +3342,7 @@
       <c r="Z40" s="2"/>
       <c r="AA40" s="2"/>
     </row>
-    <row r="41" spans="1:27" ht="72" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -3368,16 +3362,16 @@
         <v>122</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>148</v>
+        <v>138</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
@@ -31657,11 +31651,13 @@
     <hyperlink ref="J38" r:id="rId5" xr:uid="{55385EBF-5F36-49F3-9FA4-9D05AB121BDE}"/>
     <hyperlink ref="J40:J41" r:id="rId6" display="https://seng637g5.backlog.com/view/ATM_1-19" xr:uid="{57103C28-483E-4D2E-BECB-02C15AD1E755}"/>
     <hyperlink ref="J3" r:id="rId7" xr:uid="{5EAB2763-F4EC-462D-A9D5-D5AAB6182009}"/>
+    <hyperlink ref="J7" r:id="rId8" xr:uid="{AC8AE37E-22A3-42B1-8D94-A8DF612BA9DA}"/>
+    <hyperlink ref="J14" r:id="rId9" xr:uid="{315E9F15-2234-441D-BBEC-CDD58861F9AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>